<commit_message>
/ ‘LRN/LRN - contacts.xlsx’
</commit_message>
<xml_diff>
--- a/LRN/LRN - contacts.xlsx
+++ b/LRN/LRN - contacts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>ENTREPRISE</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Gilles Latouche</t>
   </si>
   <si>
-    <t>Emmanuel Lalau</t>
-  </si>
-  <si>
     <t>Jean-Michel Durand</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>Paul Rangdet</t>
   </si>
   <si>
-    <t>LM ING</t>
-  </si>
-  <si>
     <t>Ghislain Beillard</t>
   </si>
   <si>
@@ -247,6 +241,9 @@
   </si>
   <si>
     <t>FING</t>
+  </si>
+  <si>
+    <t>Julien Dugarry</t>
   </si>
 </sst>
 </file>
@@ -594,7 +591,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -620,7 +617,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -641,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
@@ -652,130 +649,128 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -783,16 +778,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -800,16 +795,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -817,43 +812,41 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -862,11 +855,11 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -875,13 +868,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -889,12 +882,14 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -904,10 +899,10 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -917,7 +912,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -928,7 +923,7 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -939,7 +934,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>

</xml_diff>